<commit_message>
report-checklist: added "GESTIONE ERRORE" for KO tests
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuvyta.sharepoint.com/sites/Developers/Documenti condivisi/FSE 2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\nuvyta-it-fse-accreditamento\GATEWAY\S1#111NUVYTA00000\nuvyta\nuplatform\2.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{93E653FA-83E9-43CF-A93F-425886593BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BF6C4DE-F6AB-4FDC-8685-E5F1ABE8AAAA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EBD1FB-3FDE-4868-94F6-F389D663B18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="171">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -892,6 +892,12 @@
   <si>
     <t>Viene inserito un log applicativo e notificato all'utente il timeout.</t>
   </si>
+  <si>
+    <t>Errore durante il processamento del documento</t>
+  </si>
+  <si>
+    <t>Viene inserito un log applicativo</t>
+  </si>
 </sst>
 </file>
 
@@ -1435,7 +1441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1567,6 +1573,41 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1608,80 +1649,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1754,10 +1724,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3130,10 +3096,10 @@
   <dimension ref="A1:T873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3179,14 +3145,14 @@
       <c r="T1" s="27"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="58"/>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
@@ -3204,14 +3170,14 @@
       <c r="T2" s="27"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="57" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="58"/>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
@@ -3229,12 +3195,12 @@
       <c r="T3" s="27"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="57" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="29"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
@@ -3253,12 +3219,12 @@
       <c r="T4" s="27"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="64"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="58"/>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -3276,8 +3242,8 @@
       <c r="T5" s="27"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="30"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -3548,27 +3514,27 @@
       <c r="E13" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="59">
+      <c r="F13" s="47">
         <v>44985</v>
       </c>
-      <c r="G13" s="60" t="s">
+      <c r="G13" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="H13" s="60" t="s">
+      <c r="H13" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="I13" s="60" t="s">
+      <c r="I13" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="J13" s="61" t="s">
+      <c r="J13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
       <c r="Q13" s="39" t="s">
         <v>86</v>
       </c>
@@ -3594,22 +3560,22 @@
       <c r="E14" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="65" t="s">
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="66" t="s">
+      <c r="K14" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="L14" s="64"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="58"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="46"/>
       <c r="R14" s="42"/>
       <c r="S14" s="40"/>
       <c r="T14" s="44" t="s">
@@ -3635,32 +3601,34 @@
       <c r="F15" s="37">
         <v>44985</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="G15" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="I15" s="62" t="s">
+      <c r="I15" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="63" t="s">
+      <c r="J15" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63" t="s">
+      <c r="K15" s="51"/>
+      <c r="L15" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="63" t="s">
+      <c r="M15" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="N15" s="63" t="s">
+      <c r="N15" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="O15" s="63" t="s">
+      <c r="O15" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="63"/>
+      <c r="P15" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q15" s="39" t="s">
         <v>86</v>
       </c>
@@ -3698,9 +3666,11 @@
         <v>88</v>
       </c>
       <c r="M16" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="N16" s="39"/>
+        <v>40</v>
+      </c>
+      <c r="N16" s="39" t="s">
+        <v>169</v>
+      </c>
       <c r="O16" s="39" t="s">
         <v>40</v>
       </c>
@@ -3760,7 +3730,9 @@
       <c r="O17" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P17" s="39"/>
+      <c r="P17" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q17" s="39" t="s">
         <v>86</v>
       </c>
@@ -3770,7 +3742,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="375.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="390.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34">
         <v>64</v>
       </c>
@@ -3814,7 +3786,9 @@
       <c r="O18" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P18" s="39"/>
+      <c r="P18" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q18" s="39" t="s">
         <v>86</v>
       </c>
@@ -3868,7 +3842,9 @@
       <c r="O19" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="39"/>
+      <c r="P19" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q19" s="39" t="s">
         <v>86</v>
       </c>
@@ -3878,7 +3854,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="34">
         <v>66</v>
       </c>
@@ -3922,7 +3898,9 @@
       <c r="O20" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P20" s="39"/>
+      <c r="P20" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q20" s="39" t="s">
         <v>86</v>
       </c>
@@ -3932,7 +3910,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="405.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34">
         <v>67</v>
       </c>
@@ -3976,7 +3954,9 @@
       <c r="O21" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P21" s="39"/>
+      <c r="P21" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q21" s="39" t="s">
         <v>86</v>
       </c>
@@ -4030,7 +4010,9 @@
       <c r="O22" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P22" s="39"/>
+      <c r="P22" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q22" s="39" t="s">
         <v>86</v>
       </c>
@@ -4084,7 +4066,9 @@
       <c r="O23" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P23" s="39"/>
+      <c r="P23" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q23" s="39" t="s">
         <v>86</v>
       </c>
@@ -4094,7 +4078,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="375.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="390.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34">
         <v>70</v>
       </c>
@@ -4138,7 +4122,9 @@
       <c r="O24" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P24" s="39"/>
+      <c r="P24" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q24" s="39" t="s">
         <v>86</v>
       </c>
@@ -4192,7 +4178,9 @@
       <c r="O25" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P25" s="39"/>
+      <c r="P25" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q25" s="39" t="s">
         <v>86</v>
       </c>
@@ -4202,41 +4190,41 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="76" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67">
+    <row r="26" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34">
         <v>72</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D26" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="69" t="s">
+      <c r="E26" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="72" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="K26" s="72" t="s">
+      <c r="K26" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="73"/>
-      <c r="S26" s="74"/>
-      <c r="T26" s="75" t="s">
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4284,7 +4272,9 @@
       <c r="O27" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="P27" s="39"/>
+      <c r="P27" s="51" t="s">
+        <v>170</v>
+      </c>
       <c r="Q27" s="39" t="s">
         <v>86</v>
       </c>
@@ -4294,41 +4284,41 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="76" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="67">
+    <row r="28" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
         <v>74</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="69" t="s">
+      <c r="E28" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="70"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="72" t="s">
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="72" t="s">
+      <c r="K28" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="L28" s="72"/>
-      <c r="M28" s="72"/>
-      <c r="N28" s="72"/>
-      <c r="O28" s="72"/>
-      <c r="P28" s="72"/>
-      <c r="Q28" s="72"/>
-      <c r="R28" s="73"/>
-      <c r="S28" s="74"/>
-      <c r="T28" s="75" t="s">
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -20899,26 +20889,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DFBE386201AE734F9EC9E17D4E3DD9C4" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="5f97ab7aa040c3457a612e608e5ad366">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce" xmlns:ns3="3560cf22-a742-4796-b196-7e41d1f38b33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47906dabeb809e6ed6721806972ae013" ns2:_="" ns3:_="">
     <xsd:import namespace="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
@@ -21161,7 +21131,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
+    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
@@ -21178,18 +21195,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}"/>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Check list file: added note to VALIDAZIONE_CDA2_RSA_CT11_KO
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\nuvyta-it-fse-accreditamento\GATEWAY\S1#111NUVYTA00000\nuvyta\nuplatform\2.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB696F2-5D27-4C35-B12F-7650E625A8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D7E37C-E371-4418-96D4-E8BD541F6848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-6250" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -1480,9 +1480,6 @@
 }</t>
   </si>
   <si>
-    <t>La risposta del servizio è HTTP422 anziché HTTP400 dichiarato nel test case</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
@@ -1572,6 +1569,9 @@
   </si>
   <si>
     <t>Fare riferimento agli "ID TEST CASE KO" del Tipo "LAB"</t>
+  </si>
+  <si>
+    <t>La risposta del servizio è HTTP422 anziché HTTP400 dichiarato nel test case. Tracciato in https://github.com/ministero-salute/it-fse-support/issues/139</t>
   </si>
 </sst>
 </file>
@@ -2124,47 +2124,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2241,6 +2200,47 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2615,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3688,11 +3688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T874"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3738,14 +3738,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="55"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3763,14 +3763,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="31"/>
+      <c r="D3" s="55"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3788,12 +3788,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="18"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -3812,12 +3812,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="39" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="55"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -3835,8 +3835,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="19"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -3954,2242 +3954,2242 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="150" x14ac:dyDescent="0.25">
-      <c r="A10" s="42">
+      <c r="A10" s="30">
         <v>6</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="32">
         <v>44985</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45" t="s">
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R10" s="46"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="45" t="s">
+      <c r="R10" s="34"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="42">
+      <c r="A11" s="30">
         <v>7</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="44">
+      <c r="F11" s="32">
         <v>44985</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45" t="s">
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R11" s="46"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="45" t="s">
+      <c r="R11" s="34"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="150" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
+      <c r="A12" s="30">
         <v>8</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="32">
         <v>44985</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="44" t="s">
+      <c r="I12" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="J12" s="45" t="s">
+      <c r="J12" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45" t="s">
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R12" s="46"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="45" t="s">
+      <c r="R12" s="34"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="150" x14ac:dyDescent="0.25">
-      <c r="A13" s="42">
+      <c r="A13" s="30">
         <v>9</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="32">
         <v>44985</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="I13" s="44" t="s">
+      <c r="I13" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="J13" s="45" t="s">
+      <c r="J13" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45" t="s">
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R13" s="46"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="45" t="s">
+      <c r="R13" s="34"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="33" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="42">
+      <c r="A14" s="30">
         <v>29</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="45" t="s">
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="45" t="s">
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="375.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42">
+      <c r="A15" s="30">
         <v>37</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="32">
         <v>44985</v>
       </c>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45" t="s">
+      <c r="K15" s="33"/>
+      <c r="L15" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N15" s="45" t="s">
+      <c r="N15" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="O15" s="45" t="s">
+      <c r="O15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P15" s="45" t="s">
+      <c r="P15" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q15" s="45" t="s">
+      <c r="Q15" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R15" s="46"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="45" t="s">
+      <c r="R15" s="34"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="375" x14ac:dyDescent="0.25">
-      <c r="A16" s="55">
+      <c r="A16" s="43">
         <v>40</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="F16" s="28">
+        <v>44992</v>
+      </c>
+      <c r="G16" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="F16" s="40">
-        <v>44992</v>
-      </c>
-      <c r="G16" s="57" t="s">
+      <c r="H16" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="H16" s="57" t="s">
+      <c r="I16" s="45" t="s">
         <v>302</v>
-      </c>
-      <c r="I16" s="57" t="s">
-        <v>303</v>
       </c>
       <c r="J16" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58" t="s">
+      <c r="K16" s="46"/>
+      <c r="L16" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="M16" s="58" t="s">
+      <c r="M16" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="N16" s="58" t="s">
-        <v>304</v>
-      </c>
-      <c r="O16" s="58" t="s">
+      <c r="N16" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="O16" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="45" t="s">
+      <c r="P16" s="33" t="s">
         <v>170</v>
       </c>
       <c r="Q16" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="R16" s="59"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="41" t="s">
+      <c r="R16" s="47"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="29" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="42">
+      <c r="A17" s="30">
         <v>45</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="45" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45" t="s">
+      <c r="K17" s="33"/>
+      <c r="L17" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M17" s="45" t="s">
+      <c r="M17" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="45" t="s">
+      <c r="N17" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="O17" s="45" t="s">
+      <c r="O17" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P17" s="45" t="s">
+      <c r="P17" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="Q17" s="45" t="s">
+      <c r="Q17" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R17" s="46"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="45" t="s">
+      <c r="R17" s="34"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A18" s="42">
+      <c r="A18" s="30">
         <v>63</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="32">
         <v>44985</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="44" t="s">
+      <c r="H18" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="44" t="s">
+      <c r="I18" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="J18" s="45" t="s">
+      <c r="J18" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45" t="s">
+      <c r="K18" s="33"/>
+      <c r="L18" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M18" s="45" t="s">
+      <c r="M18" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N18" s="45" t="s">
+      <c r="N18" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="O18" s="45" t="s">
+      <c r="O18" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P18" s="45" t="s">
+      <c r="P18" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q18" s="45" t="s">
+      <c r="Q18" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R18" s="46"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="45" t="s">
+      <c r="R18" s="34"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="375" x14ac:dyDescent="0.25">
-      <c r="A19" s="42">
+      <c r="A19" s="30">
         <v>64</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="32">
         <v>44985</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="J19" s="45" t="s">
+      <c r="J19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45" t="s">
+      <c r="K19" s="33"/>
+      <c r="L19" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M19" s="45" t="s">
+      <c r="M19" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N19" s="45" t="s">
+      <c r="N19" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="O19" s="45" t="s">
+      <c r="O19" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P19" s="45" t="s">
+      <c r="P19" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q19" s="45" t="s">
+      <c r="Q19" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R19" s="46"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="45" t="s">
+      <c r="R19" s="34"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="42">
+      <c r="A20" s="30">
         <v>65</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="32">
         <v>44985</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="J20" s="45" t="s">
+      <c r="J20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45" t="s">
+      <c r="K20" s="33"/>
+      <c r="L20" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M20" s="45" t="s">
+      <c r="M20" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N20" s="45" t="s">
+      <c r="N20" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="O20" s="45" t="s">
+      <c r="O20" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P20" s="45" t="s">
+      <c r="P20" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q20" s="45" t="s">
+      <c r="Q20" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R20" s="46"/>
-      <c r="S20" s="54"/>
-      <c r="T20" s="45" t="s">
+      <c r="R20" s="34"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="405" x14ac:dyDescent="0.25">
-      <c r="A21" s="42">
+      <c r="A21" s="30">
         <v>66</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="32">
         <v>44985</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="J21" s="45" t="s">
+      <c r="J21" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45" t="s">
+      <c r="K21" s="33"/>
+      <c r="L21" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M21" s="45" t="s">
+      <c r="M21" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N21" s="45" t="s">
+      <c r="N21" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="O21" s="45" t="s">
+      <c r="O21" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P21" s="45" t="s">
+      <c r="P21" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q21" s="45" t="s">
+      <c r="Q21" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="45" t="s">
+      <c r="R21" s="34"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="405" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
+      <c r="A22" s="30">
         <v>67</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="32">
         <v>44985</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="H22" s="44" t="s">
+      <c r="H22" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="I22" s="44" t="s">
+      <c r="I22" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="J22" s="45" t="s">
+      <c r="J22" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45" t="s">
+      <c r="K22" s="33"/>
+      <c r="L22" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M22" s="45" t="s">
+      <c r="M22" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N22" s="45" t="s">
+      <c r="N22" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="O22" s="45" t="s">
+      <c r="O22" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P22" s="45" t="s">
+      <c r="P22" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q22" s="45" t="s">
+      <c r="Q22" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R22" s="46"/>
-      <c r="S22" s="47"/>
-      <c r="T22" s="45" t="s">
+      <c r="R22" s="34"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A23" s="42">
+      <c r="A23" s="30">
         <v>68</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="32">
         <v>44985</v>
       </c>
-      <c r="G23" s="44" t="s">
+      <c r="G23" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="H23" s="44" t="s">
+      <c r="H23" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="44" t="s">
+      <c r="I23" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="J23" s="45" t="s">
+      <c r="J23" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45" t="s">
+      <c r="K23" s="33"/>
+      <c r="L23" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M23" s="45" t="s">
+      <c r="M23" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N23" s="45" t="s">
+      <c r="N23" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="O23" s="45" t="s">
+      <c r="O23" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P23" s="45" t="s">
+      <c r="P23" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q23" s="45" t="s">
+      <c r="Q23" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R23" s="46"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="45" t="s">
+      <c r="R23" s="34"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="42">
+      <c r="A24" s="30">
         <v>69</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="32">
         <v>44985</v>
       </c>
-      <c r="G24" s="44" t="s">
+      <c r="G24" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="H24" s="44" t="s">
+      <c r="H24" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="J24" s="45" t="s">
+      <c r="J24" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45" t="s">
+      <c r="K24" s="33"/>
+      <c r="L24" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M24" s="45" t="s">
+      <c r="M24" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N24" s="45" t="s">
+      <c r="N24" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="O24" s="45" t="s">
+      <c r="O24" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P24" s="45" t="s">
+      <c r="P24" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q24" s="45" t="s">
+      <c r="Q24" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R24" s="46"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="45" t="s">
+      <c r="R24" s="34"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="375" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="30">
         <v>70</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="32">
         <v>44985</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="I25" s="44" t="s">
+      <c r="I25" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="J25" s="45" t="s">
+      <c r="J25" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45" t="s">
+      <c r="K25" s="33"/>
+      <c r="L25" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M25" s="45" t="s">
+      <c r="M25" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N25" s="45" t="s">
+      <c r="N25" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="O25" s="45" t="s">
+      <c r="O25" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P25" s="45" t="s">
+      <c r="P25" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q25" s="45" t="s">
+      <c r="Q25" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R25" s="46"/>
-      <c r="S25" s="47"/>
-      <c r="T25" s="45" t="s">
+      <c r="R25" s="34"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="30">
         <v>71</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="32">
         <v>44985</v>
       </c>
-      <c r="G26" s="44" t="s">
+      <c r="G26" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="H26" s="44" t="s">
+      <c r="H26" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="I26" s="44" t="s">
+      <c r="I26" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="J26" s="45" t="s">
+      <c r="J26" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45" t="s">
+      <c r="K26" s="33"/>
+      <c r="L26" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M26" s="45" t="s">
+      <c r="M26" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N26" s="45" t="s">
+      <c r="N26" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="O26" s="45" t="s">
+      <c r="O26" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="45" t="s">
+      <c r="P26" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q26" s="45" t="s">
+      <c r="Q26" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R26" s="46"/>
-      <c r="S26" s="47"/>
-      <c r="T26" s="45" t="s">
+      <c r="R26" s="34"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A27" s="42">
+      <c r="A27" s="30">
         <v>72</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="45" t="s">
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="K27" s="45" t="s">
+      <c r="K27" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="45" t="s">
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A28" s="42">
+      <c r="A28" s="30">
         <v>73</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="43" t="s">
+      <c r="E28" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="32">
         <v>44985</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="H28" s="44" t="s">
+      <c r="H28" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I28" s="44" t="s">
+      <c r="I28" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45" t="s">
+      <c r="K28" s="33"/>
+      <c r="L28" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="M28" s="45" t="s">
+      <c r="M28" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="N28" s="45" t="s">
+      <c r="N28" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="O28" s="45" t="s">
+      <c r="O28" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="P28" s="45" t="s">
+      <c r="P28" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q28" s="45" t="s">
+      <c r="Q28" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R28" s="46"/>
-      <c r="S28" s="47"/>
-      <c r="T28" s="45" t="s">
+      <c r="R28" s="34"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
+      <c r="A29" s="30">
         <v>74</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E29" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="45" t="s">
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="45" t="s">
+      <c r="K29" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="47"/>
-      <c r="T29" s="45" t="s">
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="35"/>
+      <c r="T29" s="33" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A30" s="50">
+      <c r="A30" s="38">
         <v>147</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="52">
+      <c r="F30" s="40">
         <v>44992</v>
       </c>
-      <c r="G30" s="52" t="s">
+      <c r="G30" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="52" t="s">
+      <c r="H30" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="I30" s="52" t="s">
+      <c r="I30" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="J30" s="45" t="s">
+      <c r="J30" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="53"/>
-      <c r="P30" s="53"/>
-      <c r="Q30" s="45" t="s">
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="41"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R30" s="46"/>
+      <c r="R30" s="34"/>
       <c r="S30" s="5"/>
-      <c r="T30" s="53" t="s">
+      <c r="T30" s="41" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A31" s="50">
+      <c r="A31" s="38">
         <v>148</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="50" t="s">
+      <c r="C31" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="50" t="s">
+      <c r="D31" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="F31" s="52">
+      <c r="F31" s="40">
         <v>44992</v>
       </c>
-      <c r="G31" s="52" t="s">
+      <c r="G31" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="52" t="s">
+      <c r="H31" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I31" s="52" t="s">
+      <c r="I31" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="J31" s="45" t="s">
+      <c r="J31" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="45" t="s">
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R31" s="46"/>
+      <c r="R31" s="34"/>
       <c r="S31" s="5"/>
-      <c r="T31" s="53" t="s">
+      <c r="T31" s="41" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="50">
+      <c r="A32" s="38">
         <v>149</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="50" t="s">
+      <c r="C32" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="50" t="s">
+      <c r="D32" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="F32" s="52">
+      <c r="F32" s="40">
         <v>44992</v>
       </c>
-      <c r="G32" s="52" t="s">
+      <c r="G32" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="52" t="s">
+      <c r="H32" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="I32" s="52" t="s">
+      <c r="I32" s="40" t="s">
         <v>186</v>
       </c>
-      <c r="J32" s="45" t="s">
+      <c r="J32" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="53"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="45" t="s">
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R32" s="46"/>
+      <c r="R32" s="34"/>
       <c r="S32" s="5"/>
-      <c r="T32" s="53" t="s">
+      <c r="T32" s="41" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="50">
+      <c r="A33" s="38">
         <v>150</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C33" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D33" s="50" t="s">
+      <c r="D33" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="F33" s="52">
+      <c r="F33" s="40">
         <v>44992</v>
       </c>
-      <c r="G33" s="52" t="s">
+      <c r="G33" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="H33" s="52" t="s">
+      <c r="H33" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="I33" s="52" t="s">
+      <c r="I33" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="J33" s="45" t="s">
+      <c r="J33" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="45" t="s">
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R33" s="46"/>
+      <c r="R33" s="34"/>
       <c r="S33" s="5"/>
-      <c r="T33" s="53" t="s">
+      <c r="T33" s="41" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="50">
+      <c r="A34" s="38">
         <v>151</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="40">
         <v>44992</v>
       </c>
-      <c r="G34" s="52" t="s">
+      <c r="G34" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="H34" s="52" t="s">
+      <c r="H34" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="I34" s="52" t="s">
+      <c r="I34" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="J34" s="45" t="s">
+      <c r="J34" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53" t="s">
+      <c r="K34" s="41"/>
+      <c r="L34" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M34" s="53" t="s">
+      <c r="M34" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N34" s="53" t="s">
+      <c r="N34" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="O34" s="53" t="s">
+      <c r="O34" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P34" s="45" t="s">
+      <c r="P34" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q34" s="45" t="s">
+      <c r="Q34" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R34" s="46"/>
+      <c r="R34" s="34"/>
       <c r="S34" s="5"/>
-      <c r="T34" s="53" t="s">
+      <c r="T34" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="50">
+      <c r="A35" s="38">
         <v>152</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D35" s="50" t="s">
+      <c r="D35" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="52">
+      <c r="F35" s="40">
         <v>44992</v>
       </c>
-      <c r="G35" s="52" t="s">
+      <c r="G35" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="H35" s="52" t="s">
+      <c r="H35" s="40" t="s">
         <v>201</v>
       </c>
-      <c r="I35" s="52" t="s">
+      <c r="I35" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53" t="s">
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M35" s="53" t="s">
+      <c r="M35" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N35" s="53" t="s">
+      <c r="N35" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="O35" s="53" t="s">
+      <c r="O35" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P35" s="45" t="s">
+      <c r="P35" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="46"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="34"/>
       <c r="S35" s="5"/>
-      <c r="T35" s="53" t="s">
+      <c r="T35" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="50">
+      <c r="A36" s="38">
         <v>153</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D36" s="50" t="s">
+      <c r="D36" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="40">
         <v>44992</v>
       </c>
-      <c r="G36" s="52" t="s">
+      <c r="G36" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="H36" s="52" t="s">
+      <c r="H36" s="40" t="s">
         <v>207</v>
       </c>
-      <c r="I36" s="52" t="s">
+      <c r="I36" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="J36" s="45" t="s">
+      <c r="J36" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53" t="s">
+      <c r="K36" s="41"/>
+      <c r="L36" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M36" s="53" t="s">
+      <c r="M36" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N36" s="53" t="s">
+      <c r="N36" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="O36" s="53" t="s">
+      <c r="O36" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P36" s="45" t="s">
+      <c r="P36" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q36" s="45" t="s">
+      <c r="Q36" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R36" s="46"/>
+      <c r="R36" s="34"/>
       <c r="S36" s="5"/>
-      <c r="T36" s="53" t="s">
+      <c r="T36" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="405" x14ac:dyDescent="0.25">
-      <c r="A37" s="50">
+      <c r="A37" s="38">
         <v>154</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="F37" s="52">
+      <c r="F37" s="40">
         <v>44992</v>
       </c>
-      <c r="G37" s="52" t="s">
+      <c r="G37" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="H37" s="52" t="s">
+      <c r="H37" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="I37" s="52" t="s">
+      <c r="I37" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="J37" s="53" t="s">
+      <c r="J37" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53" t="s">
+      <c r="K37" s="41"/>
+      <c r="L37" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M37" s="53" t="s">
+      <c r="M37" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N37" s="53" t="s">
+      <c r="N37" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="O37" s="53" t="s">
+      <c r="O37" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P37" s="45" t="s">
+      <c r="P37" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q37" s="45" t="s">
+      <c r="Q37" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="R37" s="46"/>
+      <c r="R37" s="34"/>
       <c r="S37" s="5"/>
-      <c r="T37" s="53" t="s">
+      <c r="T37" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="405" x14ac:dyDescent="0.25">
-      <c r="A38" s="50">
+      <c r="A38" s="38">
         <v>155</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="F38" s="52">
+      <c r="F38" s="40">
         <v>44992</v>
       </c>
-      <c r="G38" s="52" t="s">
+      <c r="G38" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="H38" s="52" t="s">
+      <c r="H38" s="40" t="s">
         <v>219</v>
       </c>
-      <c r="I38" s="52" t="s">
+      <c r="I38" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="J38" s="53" t="s">
+      <c r="J38" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53" t="s">
+      <c r="K38" s="41"/>
+      <c r="L38" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M38" s="53" t="s">
+      <c r="M38" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N38" s="53" t="s">
+      <c r="N38" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="O38" s="53" t="s">
+      <c r="O38" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P38" s="45" t="s">
+      <c r="P38" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q38" s="53" t="s">
+      <c r="Q38" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R38" s="46"/>
+      <c r="R38" s="34"/>
       <c r="S38" s="5"/>
-      <c r="T38" s="53" t="s">
+      <c r="T38" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A39" s="50">
+      <c r="A39" s="38">
         <v>156</v>
       </c>
-      <c r="B39" s="50" t="s">
+      <c r="B39" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="C39" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="50" t="s">
+      <c r="D39" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="E39" s="51" t="s">
+      <c r="E39" s="39" t="s">
         <v>223</v>
       </c>
-      <c r="F39" s="52">
+      <c r="F39" s="40">
         <v>44992</v>
       </c>
-      <c r="G39" s="52" t="s">
+      <c r="G39" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="H39" s="52" t="s">
+      <c r="H39" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="I39" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="J39" s="53" t="s">
+      <c r="J39" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53" t="s">
+      <c r="K39" s="41"/>
+      <c r="L39" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M39" s="53" t="s">
+      <c r="M39" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N39" s="53" t="s">
+      <c r="N39" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="O39" s="53" t="s">
+      <c r="O39" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P39" s="45" t="s">
+      <c r="P39" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q39" s="53" t="s">
+      <c r="Q39" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R39" s="46"/>
+      <c r="R39" s="34"/>
       <c r="S39" s="5"/>
-      <c r="T39" s="53" t="s">
+      <c r="T39" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="50">
+      <c r="A40" s="38">
         <v>157</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D40" s="50" t="s">
+      <c r="D40" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="40">
         <v>44992</v>
       </c>
-      <c r="G40" s="52" t="s">
+      <c r="G40" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="H40" s="52" t="s">
+      <c r="H40" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="I40" s="52" t="s">
+      <c r="I40" s="40" t="s">
         <v>232</v>
       </c>
-      <c r="J40" s="53" t="s">
+      <c r="J40" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53" t="s">
+      <c r="K40" s="41"/>
+      <c r="L40" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M40" s="53" t="s">
+      <c r="M40" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N40" s="53" t="s">
+      <c r="N40" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="O40" s="53" t="s">
+      <c r="O40" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P40" s="45" t="s">
+      <c r="P40" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q40" s="53" t="s">
+      <c r="Q40" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R40" s="46"/>
-      <c r="S40" s="51" t="s">
-        <v>298</v>
-      </c>
-      <c r="T40" s="53" t="s">
+      <c r="R40" s="34"/>
+      <c r="S40" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="T40" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="50">
+      <c r="A41" s="38">
         <v>158</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="50" t="s">
+      <c r="C41" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D41" s="50" t="s">
+      <c r="D41" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="F41" s="52">
+      <c r="F41" s="40">
         <v>44992</v>
       </c>
-      <c r="G41" s="52" t="s">
+      <c r="G41" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="H41" s="52" t="s">
+      <c r="H41" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="I41" s="52" t="s">
+      <c r="I41" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="J41" s="53" t="s">
+      <c r="J41" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53" t="s">
+      <c r="K41" s="41"/>
+      <c r="L41" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M41" s="53" t="s">
+      <c r="M41" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N41" s="53" t="s">
+      <c r="N41" s="41" t="s">
         <v>239</v>
       </c>
-      <c r="O41" s="53" t="s">
+      <c r="O41" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P41" s="45" t="s">
+      <c r="P41" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q41" s="53" t="s">
+      <c r="Q41" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R41" s="46"/>
+      <c r="R41" s="34"/>
       <c r="S41" s="5"/>
-      <c r="T41" s="53" t="s">
+      <c r="T41" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="50">
+      <c r="A42" s="38">
         <v>159</v>
       </c>
-      <c r="B42" s="50" t="s">
+      <c r="B42" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="50" t="s">
+      <c r="C42" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D42" s="50" t="s">
+      <c r="D42" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="E42" s="51" t="s">
+      <c r="E42" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="F42" s="52">
+      <c r="F42" s="40">
         <v>44992</v>
       </c>
-      <c r="G42" s="52" t="s">
+      <c r="G42" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="H42" s="52" t="s">
+      <c r="H42" s="40" t="s">
         <v>243</v>
       </c>
-      <c r="I42" s="52" t="s">
+      <c r="I42" s="40" t="s">
         <v>244</v>
       </c>
-      <c r="J42" s="53" t="s">
+      <c r="J42" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53" t="s">
+      <c r="K42" s="41"/>
+      <c r="L42" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M42" s="53" t="s">
+      <c r="M42" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N42" s="53" t="s">
+      <c r="N42" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="O42" s="53" t="s">
+      <c r="O42" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P42" s="45" t="s">
+      <c r="P42" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q42" s="53" t="s">
+      <c r="Q42" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R42" s="46"/>
+      <c r="R42" s="34"/>
       <c r="S42" s="5"/>
-      <c r="T42" s="53" t="s">
+      <c r="T42" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="50">
+      <c r="A43" s="38">
         <v>160</v>
       </c>
-      <c r="B43" s="50" t="s">
+      <c r="B43" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="50" t="s">
+      <c r="C43" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D43" s="50" t="s">
+      <c r="D43" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="E43" s="51" t="s">
+      <c r="E43" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="F43" s="52">
+      <c r="F43" s="40">
         <v>44992</v>
       </c>
-      <c r="G43" s="52" t="s">
+      <c r="G43" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="H43" s="52" t="s">
+      <c r="H43" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="I43" s="52" t="s">
+      <c r="I43" s="40" t="s">
         <v>250</v>
       </c>
-      <c r="J43" s="53" t="s">
+      <c r="J43" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53" t="s">
+      <c r="K43" s="41"/>
+      <c r="L43" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M43" s="53" t="s">
+      <c r="M43" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N43" s="53" t="s">
+      <c r="N43" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="O43" s="53" t="s">
+      <c r="O43" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P43" s="45" t="s">
+      <c r="P43" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q43" s="53" t="s">
+      <c r="Q43" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R43" s="46"/>
+      <c r="R43" s="34"/>
       <c r="S43" s="5"/>
-      <c r="T43" s="53" t="s">
+      <c r="T43" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="405" x14ac:dyDescent="0.25">
-      <c r="A44" s="50">
+      <c r="A44" s="38">
         <v>161</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="50" t="s">
+      <c r="C44" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="F44" s="52">
+      <c r="F44" s="40">
         <v>44992</v>
       </c>
-      <c r="G44" s="52" t="s">
+      <c r="G44" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="H44" s="52" t="s">
+      <c r="H44" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="I44" s="52" t="s">
+      <c r="I44" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="J44" s="53" t="s">
+      <c r="J44" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53" t="s">
+      <c r="K44" s="41"/>
+      <c r="L44" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M44" s="53" t="s">
+      <c r="M44" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N44" s="53" t="s">
+      <c r="N44" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="O44" s="53" t="s">
+      <c r="O44" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P44" s="45" t="s">
+      <c r="P44" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q44" s="53" t="s">
+      <c r="Q44" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R44" s="46"/>
+      <c r="R44" s="34"/>
       <c r="S44" s="5"/>
-      <c r="T44" s="53" t="s">
+      <c r="T44" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="375" x14ac:dyDescent="0.25">
-      <c r="A45" s="50">
+      <c r="A45" s="38">
         <v>162</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="50" t="s">
+      <c r="C45" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D45" s="50" t="s">
+      <c r="D45" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="F45" s="52">
+      <c r="F45" s="40">
         <v>44992</v>
       </c>
-      <c r="G45" s="52" t="s">
+      <c r="G45" s="40" t="s">
         <v>260</v>
       </c>
-      <c r="H45" s="52" t="s">
+      <c r="H45" s="40" t="s">
         <v>261</v>
       </c>
-      <c r="I45" s="52" t="s">
+      <c r="I45" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="J45" s="53" t="s">
+      <c r="J45" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53" t="s">
+      <c r="K45" s="41"/>
+      <c r="L45" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M45" s="53" t="s">
+      <c r="M45" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="53" t="s">
+      <c r="N45" s="41" t="s">
         <v>263</v>
       </c>
-      <c r="O45" s="53" t="s">
+      <c r="O45" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P45" s="45" t="s">
+      <c r="P45" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q45" s="53" t="s">
+      <c r="Q45" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R45" s="46"/>
+      <c r="R45" s="34"/>
       <c r="S45" s="5"/>
-      <c r="T45" s="53" t="s">
+      <c r="T45" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="360" x14ac:dyDescent="0.25">
-      <c r="A46" s="50">
+      <c r="A46" s="38">
         <v>163</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="50" t="s">
+      <c r="C46" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D46" s="50" t="s">
+      <c r="D46" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="E46" s="51" t="s">
+      <c r="E46" s="39" t="s">
         <v>265</v>
       </c>
-      <c r="F46" s="52">
+      <c r="F46" s="40">
         <v>44992</v>
       </c>
-      <c r="G46" s="52" t="s">
+      <c r="G46" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="H46" s="52" t="s">
+      <c r="H46" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="I46" s="52" t="s">
+      <c r="I46" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="J46" s="53" t="s">
+      <c r="J46" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K46" s="53"/>
-      <c r="L46" s="53" t="s">
+      <c r="K46" s="41"/>
+      <c r="L46" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M46" s="53" t="s">
+      <c r="M46" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N46" s="53" t="s">
+      <c r="N46" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="O46" s="53" t="s">
+      <c r="O46" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P46" s="45" t="s">
+      <c r="P46" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q46" s="53" t="s">
+      <c r="Q46" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R46" s="46"/>
+      <c r="R46" s="34"/>
       <c r="S46" s="5"/>
-      <c r="T46" s="53" t="s">
+      <c r="T46" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="50">
+      <c r="A47" s="38">
         <v>164</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="50" t="s">
+      <c r="C47" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="E47" s="51" t="s">
+      <c r="E47" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="F47" s="52">
+      <c r="F47" s="40">
         <v>44992</v>
       </c>
-      <c r="G47" s="52" t="s">
+      <c r="G47" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="H47" s="52" t="s">
+      <c r="H47" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="I47" s="52" t="s">
+      <c r="I47" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="J47" s="53" t="s">
+      <c r="J47" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53" t="s">
+      <c r="K47" s="41"/>
+      <c r="L47" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M47" s="53" t="s">
+      <c r="M47" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N47" s="53" t="s">
+      <c r="N47" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="O47" s="53" t="s">
+      <c r="O47" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P47" s="45" t="s">
+      <c r="P47" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q47" s="53" t="s">
+      <c r="Q47" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R47" s="46"/>
+      <c r="R47" s="34"/>
       <c r="S47" s="5"/>
-      <c r="T47" s="53" t="s">
+      <c r="T47" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="50">
+      <c r="A48" s="38">
         <v>165</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D48" s="50" t="s">
+      <c r="D48" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="E48" s="51" t="s">
+      <c r="E48" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="F48" s="52">
+      <c r="F48" s="40">
         <v>44992</v>
       </c>
-      <c r="G48" s="52" t="s">
+      <c r="G48" s="40" t="s">
         <v>278</v>
       </c>
-      <c r="H48" s="52" t="s">
+      <c r="H48" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="I48" s="52" t="s">
+      <c r="I48" s="40" t="s">
         <v>280</v>
       </c>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53" t="s">
+      <c r="J48" s="41"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M48" s="53" t="s">
+      <c r="M48" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N48" s="53" t="s">
+      <c r="N48" s="41" t="s">
         <v>281</v>
       </c>
-      <c r="O48" s="53" t="s">
+      <c r="O48" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P48" s="45" t="s">
+      <c r="P48" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q48" s="53"/>
-      <c r="R48" s="46"/>
+      <c r="Q48" s="41"/>
+      <c r="R48" s="34"/>
       <c r="S48" s="5"/>
-      <c r="T48" s="53" t="s">
+      <c r="T48" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="135" x14ac:dyDescent="0.25">
-      <c r="A49" s="50">
+      <c r="A49" s="38">
         <v>166</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="E49" s="51" t="s">
+      <c r="E49" s="39" t="s">
         <v>283</v>
       </c>
-      <c r="F49" s="52"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="53" t="s">
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="K49" s="45" t="s">
+      <c r="K49" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="L49" s="53" t="s">
+      <c r="L49" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M49" s="53" t="s">
+      <c r="M49" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N49" s="53"/>
-      <c r="O49" s="53" t="s">
+      <c r="N49" s="41"/>
+      <c r="O49" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P49" s="45" t="s">
+      <c r="P49" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q49" s="53"/>
-      <c r="R49" s="46"/>
+      <c r="Q49" s="41"/>
+      <c r="R49" s="34"/>
       <c r="S49" s="5"/>
-      <c r="T49" s="53" t="s">
+      <c r="T49" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="135" x14ac:dyDescent="0.25">
-      <c r="A50" s="50">
+      <c r="A50" s="38">
         <v>167</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="50" t="s">
+      <c r="C50" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="E50" s="51" t="s">
+      <c r="E50" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="53" t="s">
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="K50" s="45" t="s">
+      <c r="K50" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="L50" s="53" t="s">
+      <c r="L50" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M50" s="53" t="s">
+      <c r="M50" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53" t="s">
+      <c r="N50" s="41"/>
+      <c r="O50" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P50" s="45" t="s">
+      <c r="P50" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="46"/>
+      <c r="Q50" s="41"/>
+      <c r="R50" s="34"/>
       <c r="S50" s="5"/>
-      <c r="T50" s="53" t="s">
+      <c r="T50" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A51" s="50">
+      <c r="A51" s="38">
         <v>168</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="E51" s="51" t="s">
+      <c r="E51" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="F51" s="52">
+      <c r="F51" s="40">
         <v>44992</v>
       </c>
-      <c r="G51" s="52" t="s">
+      <c r="G51" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="H51" s="52" t="s">
+      <c r="H51" s="40" t="s">
         <v>289</v>
       </c>
-      <c r="I51" s="52" t="s">
+      <c r="I51" s="40" t="s">
         <v>290</v>
       </c>
-      <c r="J51" s="53" t="s">
+      <c r="J51" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K51" s="53"/>
-      <c r="L51" s="53" t="s">
+      <c r="K51" s="41"/>
+      <c r="L51" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M51" s="53" t="s">
+      <c r="M51" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N51" s="53" t="s">
+      <c r="N51" s="41" t="s">
         <v>291</v>
       </c>
-      <c r="O51" s="53" t="s">
+      <c r="O51" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P51" s="45" t="s">
+      <c r="P51" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q51" s="53" t="s">
+      <c r="Q51" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R51" s="46"/>
+      <c r="R51" s="34"/>
       <c r="S51" s="5"/>
-      <c r="T51" s="53" t="s">
+      <c r="T51" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="390" x14ac:dyDescent="0.25">
-      <c r="A52" s="50">
+      <c r="A52" s="38">
         <v>169</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="50" t="s">
+      <c r="C52" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="38" t="s">
         <v>292</v>
       </c>
-      <c r="E52" s="51" t="s">
+      <c r="E52" s="39" t="s">
         <v>293</v>
       </c>
-      <c r="F52" s="52">
+      <c r="F52" s="40">
         <v>44992</v>
       </c>
-      <c r="G52" s="52" t="s">
+      <c r="G52" s="40" t="s">
         <v>294</v>
       </c>
-      <c r="H52" s="52" t="s">
+      <c r="H52" s="40" t="s">
         <v>295</v>
       </c>
-      <c r="I52" s="52" t="s">
+      <c r="I52" s="40" t="s">
         <v>296</v>
       </c>
-      <c r="J52" s="53" t="s">
+      <c r="J52" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K52" s="53"/>
-      <c r="L52" s="53" t="s">
+      <c r="K52" s="41"/>
+      <c r="L52" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="M52" s="53" t="s">
+      <c r="M52" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="N52" s="53" t="s">
+      <c r="N52" s="41" t="s">
         <v>297</v>
       </c>
-      <c r="O52" s="53" t="s">
+      <c r="O52" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="P52" s="45" t="s">
+      <c r="P52" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="Q52" s="53" t="s">
+      <c r="Q52" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="R52" s="46"/>
+      <c r="R52" s="34"/>
       <c r="S52" s="5"/>
-      <c r="T52" s="53" t="s">
+      <c r="T52" s="41" t="s">
         <v>97</v>
       </c>
     </row>
@@ -20241,129 +20241,129 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="50" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="50" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="51" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="50" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="51" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="51" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="51" t="s">
         <v>305</v>
       </c>
-      <c r="D8" s="63" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="B9" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="D9" s="51" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
+        <v>309</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="62" t="s">
-        <v>308</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+      <c r="C10" s="50">
+        <v>191</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>310</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="62">
-        <v>191</v>
-      </c>
-      <c r="D10" s="62" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22408,6 +22408,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DFBE386201AE734F9EC9E17D4E3DD9C4" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="5f97ab7aa040c3457a612e608e5ad366">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce" xmlns:ns3="3560cf22-a742-4796-b196-7e41d1f38b33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47906dabeb809e6ed6721806972ae013" ns2:_="" ns3:_="">
     <xsd:import namespace="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
@@ -22650,41 +22670,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
-    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22707,9 +22696,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
+    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed merged rows in Excel files
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\nuvyta-it-fse-accreditamento\GATEWAY\S1#111NUVYTA00000\nuvyta\nuplatform\2.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7B863A-8679-4133-B0B9-8E29D1BB933A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2942A3B-B5FB-4ED7-B83A-5A5E9A753211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="303">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1505,19 +1505,45 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855.3062a725e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.</t>
-  </si>
-  <si>
-    <t>Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-03-14T13:54:20.431Z</t>
-  </si>
-  <si>
-    <t>f0d4aaf30c5bfe16</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855.197dc200d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>VALIDAZIONE_CDA2_RSA_CT2</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t>2023-03-07T14:00:52.367Z</t>
+  </si>
+  <si>
+    <t>8c5e0e5cfcbc8ab2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855.f7709c1d5d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_RSA_CT4</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1687,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1903,11 +1929,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2045,32 +2099,11 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2112,6 +2145,58 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3559,7 +3644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T874"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -3609,14 +3694,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="50"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3634,14 +3719,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="65" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="57"/>
+      <c r="D3" s="50"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3659,12 +3744,12 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="65" t="s">
+      <c r="A4" s="54"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="18"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -3683,12 +3768,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="50"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -3706,8 +3791,8 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="19"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -4754,7 +4839,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="390" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>73</v>
       </c>
@@ -4810,7 +4895,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29">
         <v>74</v>
       </c>
@@ -4848,119 +4933,169 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52">
+    <row r="30" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="59">
         <v>147</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="53">
-        <v>44999</v>
-      </c>
-      <c r="G30" s="49" t="s">
+      <c r="E30" s="61" t="s">
         <v>295</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="F30" s="62">
+        <v>44992</v>
+      </c>
+      <c r="G30" s="63" t="s">
         <v>296</v>
       </c>
-      <c r="I30" s="49" t="s">
+      <c r="H30" s="63" t="s">
         <v>297</v>
       </c>
-      <c r="J30" s="49" t="s">
+      <c r="I30" s="63" t="s">
+        <v>298</v>
+      </c>
+      <c r="J30" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49" t="s">
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="R30" s="49"/>
-      <c r="S30" s="50"/>
-      <c r="T30" s="51" t="s">
+      <c r="R30" s="66"/>
+      <c r="S30" s="67"/>
+      <c r="T30" s="68" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="46" t="s">
+    <row r="31" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="59">
+        <v>148</v>
+      </c>
+      <c r="B31" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D31" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="F31" s="53"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="51"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="51"/>
-    </row>
-    <row r="33" spans="1:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="46" t="s">
+      <c r="E31" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="F31" s="62"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="K31" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="R31" s="66"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="59">
+        <v>149</v>
+      </c>
+      <c r="B32" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D32" s="60" t="s">
         <v>294</v>
       </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="51"/>
+      <c r="E32" s="61" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="K32" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="R32" s="66"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+      <c r="A33" s="69">
+        <v>150</v>
+      </c>
+      <c r="B33" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D33" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="E33" s="70" t="s">
+        <v>301</v>
+      </c>
+      <c r="F33" s="72"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="K33" s="73" t="s">
+        <v>158</v>
+      </c>
+      <c r="L33" s="73"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="73"/>
+      <c r="O33" s="73"/>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="74"/>
+      <c r="T33" s="75" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
@@ -4975,7 +5110,7 @@
       <c r="D34" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="45" t="s">
         <v>171</v>
       </c>
       <c r="F34" s="41">
@@ -5013,12 +5148,12 @@
         <v>86</v>
       </c>
       <c r="R34" s="36"/>
-      <c r="S34" s="48"/>
+      <c r="S34" s="46"/>
       <c r="T34" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>152</v>
       </c>
@@ -5031,7 +5166,7 @@
       <c r="D35" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="45" t="s">
         <v>177</v>
       </c>
       <c r="F35" s="41">
@@ -5067,7 +5202,7 @@
       </c>
       <c r="Q35" s="42"/>
       <c r="R35" s="36"/>
-      <c r="S35" s="48"/>
+      <c r="S35" s="46"/>
       <c r="T35" s="42" t="s">
         <v>97</v>
       </c>
@@ -5085,7 +5220,7 @@
       <c r="D36" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="45" t="s">
         <v>183</v>
       </c>
       <c r="F36" s="41">
@@ -5123,7 +5258,7 @@
         <v>86</v>
       </c>
       <c r="R36" s="36"/>
-      <c r="S36" s="48"/>
+      <c r="S36" s="46"/>
       <c r="T36" s="42" t="s">
         <v>97</v>
       </c>
@@ -5141,7 +5276,7 @@
       <c r="D37" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="45" t="s">
         <v>189</v>
       </c>
       <c r="F37" s="41">
@@ -5179,12 +5314,12 @@
         <v>86</v>
       </c>
       <c r="R37" s="36"/>
-      <c r="S37" s="48"/>
+      <c r="S37" s="46"/>
       <c r="T37" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="405" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="405" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>155</v>
       </c>
@@ -5197,7 +5332,7 @@
       <c r="D38" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="45" t="s">
         <v>195</v>
       </c>
       <c r="F38" s="41">
@@ -5235,12 +5370,12 @@
         <v>86</v>
       </c>
       <c r="R38" s="36"/>
-      <c r="S38" s="48"/>
+      <c r="S38" s="46"/>
       <c r="T38" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="390" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>156</v>
       </c>
@@ -5253,7 +5388,7 @@
       <c r="D39" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E39" s="45" t="s">
         <v>201</v>
       </c>
       <c r="F39" s="41">
@@ -5291,7 +5426,7 @@
         <v>86</v>
       </c>
       <c r="R39" s="36"/>
-      <c r="S39" s="48"/>
+      <c r="S39" s="46"/>
       <c r="T39" s="42" t="s">
         <v>97</v>
       </c>
@@ -5309,7 +5444,7 @@
       <c r="D40" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="45" t="s">
         <v>207</v>
       </c>
       <c r="F40" s="41">
@@ -5347,7 +5482,7 @@
         <v>86</v>
       </c>
       <c r="R40" s="36"/>
-      <c r="S40" s="47" t="s">
+      <c r="S40" s="45" t="s">
         <v>289</v>
       </c>
       <c r="T40" s="42" t="s">
@@ -5367,7 +5502,7 @@
       <c r="D41" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="E41" s="47" t="s">
+      <c r="E41" s="45" t="s">
         <v>213</v>
       </c>
       <c r="F41" s="41">
@@ -5405,7 +5540,7 @@
         <v>86</v>
       </c>
       <c r="R41" s="36"/>
-      <c r="S41" s="48"/>
+      <c r="S41" s="46"/>
       <c r="T41" s="42" t="s">
         <v>97</v>
       </c>
@@ -5423,7 +5558,7 @@
       <c r="D42" s="40" t="s">
         <v>218</v>
       </c>
-      <c r="E42" s="47" t="s">
+      <c r="E42" s="45" t="s">
         <v>219</v>
       </c>
       <c r="F42" s="41">
@@ -5461,7 +5596,7 @@
         <v>86</v>
       </c>
       <c r="R42" s="36"/>
-      <c r="S42" s="48"/>
+      <c r="S42" s="46"/>
       <c r="T42" s="42" t="s">
         <v>97</v>
       </c>
@@ -5479,7 +5614,7 @@
       <c r="D43" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="45" t="s">
         <v>225</v>
       </c>
       <c r="F43" s="41">
@@ -5517,12 +5652,12 @@
         <v>86</v>
       </c>
       <c r="R43" s="36"/>
-      <c r="S43" s="48"/>
+      <c r="S43" s="46"/>
       <c r="T43" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="405" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="390" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>161</v>
       </c>
@@ -5535,7 +5670,7 @@
       <c r="D44" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="E44" s="47" t="s">
+      <c r="E44" s="45" t="s">
         <v>231</v>
       </c>
       <c r="F44" s="41">
@@ -5573,7 +5708,7 @@
         <v>86</v>
       </c>
       <c r="R44" s="36"/>
-      <c r="S44" s="48"/>
+      <c r="S44" s="46"/>
       <c r="T44" s="42" t="s">
         <v>97</v>
       </c>
@@ -5591,7 +5726,7 @@
       <c r="D45" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="E45" s="47" t="s">
+      <c r="E45" s="45" t="s">
         <v>237</v>
       </c>
       <c r="F45" s="41">
@@ -5629,12 +5764,12 @@
         <v>86</v>
       </c>
       <c r="R45" s="36"/>
-      <c r="S45" s="48"/>
+      <c r="S45" s="46"/>
       <c r="T45" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="360" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="345" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>163</v>
       </c>
@@ -5647,7 +5782,7 @@
       <c r="D46" s="40" t="s">
         <v>242</v>
       </c>
-      <c r="E46" s="47" t="s">
+      <c r="E46" s="45" t="s">
         <v>243</v>
       </c>
       <c r="F46" s="41">
@@ -5685,12 +5820,12 @@
         <v>86</v>
       </c>
       <c r="R46" s="36"/>
-      <c r="S46" s="48"/>
+      <c r="S46" s="46"/>
       <c r="T46" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="405" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>164</v>
       </c>
@@ -5703,7 +5838,7 @@
       <c r="D47" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="E47" s="47" t="s">
+      <c r="E47" s="45" t="s">
         <v>249</v>
       </c>
       <c r="F47" s="41">
@@ -5741,7 +5876,7 @@
         <v>86</v>
       </c>
       <c r="R47" s="36"/>
-      <c r="S47" s="48"/>
+      <c r="S47" s="46"/>
       <c r="T47" s="42" t="s">
         <v>97</v>
       </c>
@@ -5759,7 +5894,7 @@
       <c r="D48" s="40" t="s">
         <v>254</v>
       </c>
-      <c r="E48" s="47" t="s">
+      <c r="E48" s="45" t="s">
         <v>255</v>
       </c>
       <c r="F48" s="41">
@@ -5795,7 +5930,7 @@
       </c>
       <c r="Q48" s="42"/>
       <c r="R48" s="36"/>
-      <c r="S48" s="48"/>
+      <c r="S48" s="46"/>
       <c r="T48" s="42" t="s">
         <v>97</v>
       </c>
@@ -5813,7 +5948,7 @@
       <c r="D49" s="40" t="s">
         <v>260</v>
       </c>
-      <c r="E49" s="47" t="s">
+      <c r="E49" s="45" t="s">
         <v>261</v>
       </c>
       <c r="F49" s="41"/>
@@ -5841,7 +5976,7 @@
       </c>
       <c r="Q49" s="42"/>
       <c r="R49" s="36"/>
-      <c r="S49" s="48"/>
+      <c r="S49" s="46"/>
       <c r="T49" s="42" t="s">
         <v>97</v>
       </c>
@@ -5859,7 +5994,7 @@
       <c r="D50" s="40" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="E50" s="45" t="s">
         <v>263</v>
       </c>
       <c r="F50" s="41"/>
@@ -5887,12 +6022,12 @@
       </c>
       <c r="Q50" s="42"/>
       <c r="R50" s="36"/>
-      <c r="S50" s="48"/>
+      <c r="S50" s="46"/>
       <c r="T50" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="390" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>168</v>
       </c>
@@ -5905,7 +6040,7 @@
       <c r="D51" s="40" t="s">
         <v>264</v>
       </c>
-      <c r="E51" s="47" t="s">
+      <c r="E51" s="45" t="s">
         <v>265</v>
       </c>
       <c r="F51" s="41">
@@ -5943,12 +6078,12 @@
         <v>86</v>
       </c>
       <c r="R51" s="36"/>
-      <c r="S51" s="48"/>
+      <c r="S51" s="46"/>
       <c r="T51" s="42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="390" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>169</v>
       </c>
@@ -5961,7 +6096,7 @@
       <c r="D52" s="40" t="s">
         <v>270</v>
       </c>
-      <c r="E52" s="47" t="s">
+      <c r="E52" s="45" t="s">
         <v>271</v>
       </c>
       <c r="F52" s="41">
@@ -5999,7 +6134,7 @@
         <v>86</v>
       </c>
       <c r="R52" s="36"/>
-      <c r="S52" s="48"/>
+      <c r="S52" s="46"/>
       <c r="T52" s="42" t="s">
         <v>97</v>
       </c>
@@ -19980,7 +20115,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T52" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <mergeCells count="26">
+  <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
@@ -19988,32 +20123,13 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="G30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="J30:J33"/>
-    <mergeCell ref="K30:K33"/>
-    <mergeCell ref="Q30:Q33"/>
-    <mergeCell ref="R30:R33"/>
-    <mergeCell ref="S30:S33"/>
-    <mergeCell ref="T30:T33"/>
-    <mergeCell ref="L30:L33"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="N30:N33"/>
-    <mergeCell ref="O30:O33"/>
-    <mergeCell ref="P30:P33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7251B2DD-EAA3-474F-9C39-00147BB6DBBD}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
@@ -22238,26 +22354,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DFBE386201AE734F9EC9E17D4E3DD9C4" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="5f97ab7aa040c3457a612e608e5ad366">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce" xmlns:ns3="3560cf22-a742-4796-b196-7e41d1f38b33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47906dabeb809e6ed6721806972ae013" ns2:_="" ns3:_="">
     <xsd:import namespace="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
@@ -22500,32 +22596,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22544,6 +22635,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Added error management indications
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
+++ b/GATEWAY/S1#111NUVYTA00000/nuvyta/nuplatform/2.4/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xpira\Desktop\clone-repo-git-accreditamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\nuvyta-it-fse-accreditamento\GATEWAY\S1#111NUVYTA00000\nuvyta\nuplatform\2.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCEE66C-B772-40A3-8756-A3B75A88CB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACE526E-3E1C-4C93-AD28-65602DEDECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="2070" windowWidth="33390" windowHeight="16995" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-6250" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="305">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -505,9 +505,6 @@
 }</t>
   </si>
   <si>
-    <t>Viene inserito un log applicativo</t>
-  </si>
-  <si>
     <t>RSA</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>Errore durante il processamento del documento</t>
   </si>
   <si>
-    <t>Viene inserito un log applicativo e notificato all'utente il timeout.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
   </si>
   <si>
@@ -1544,6 +1538,18 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.e3b0c44298fc1c149afbf4c8996fb92427ae41e4649b934ca495991b7852b855.d1f03cc6fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il documento non viene inviato e gestito manualmente in backoffice dall'operatore che provvederà ad identificare e correggere eventuare anomalie o errori di configurazioni e sottometterlo manualmente</t>
+  </si>
+  <si>
+    <t>Il documento non viene inviato. L'operatore in backoffice provvederà a identificare e correggere i dati relativi al paziente e notificare al personale clinico che è necessario annullare e generare un nuovo documento dal contenuto corretto.</t>
+  </si>
+  <si>
+    <t>Il documento non viene inviato. L'operatore in backoffice provvederà a identificare e correggere le configurazioni e notificare al personale clinico che è necessario annullare e generare un nuovo documento dal contenuto corretto.</t>
+  </si>
+  <si>
+    <t>Il documento non viene inviato. L'operatore in backoffice provvederà a identificare e correggere le configurazioni o dati e notificare al personale clinico che è necessario annullare e generare un nuovo documento dal contenuto corretto.</t>
   </si>
 </sst>
 </file>
@@ -2130,6 +2136,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2171,12 +2180,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2470,7 +2476,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3621,10 +3627,10 @@
   <dimension ref="A1:T874"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3670,14 +3676,14 @@
       <c r="T1" s="13"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="66"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3695,14 +3701,14 @@
       <c r="T2" s="13"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="73" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="66"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3720,12 +3726,12 @@
       <c r="T3" s="13"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="73" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="15"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3744,12 +3750,12 @@
       <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="66"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3767,8 +3773,8 @@
       <c r="T5" s="13"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -3905,13 +3911,13 @@
         <v>45029</v>
       </c>
       <c r="G10" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>299</v>
+      </c>
+      <c r="I10" s="28" t="s">
         <v>300</v>
-      </c>
-      <c r="H10" s="74" t="s">
-        <v>301</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>302</v>
       </c>
       <c r="J10" s="28" t="s">
         <v>48</v>
@@ -3921,7 +3927,7 @@
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="P10" s="38"/>
       <c r="Q10" s="28" t="s">
         <v>49</v>
       </c>
@@ -3969,7 +3975,7 @@
       <c r="M11" s="31"/>
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
-      <c r="P11" s="31"/>
+      <c r="P11" s="38"/>
       <c r="Q11" s="31" t="s">
         <v>49</v>
       </c>
@@ -4017,7 +4023,7 @@
       <c r="M12" s="31"/>
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
-      <c r="P12" s="31"/>
+      <c r="P12" s="38"/>
       <c r="Q12" s="31" t="s">
         <v>49</v>
       </c>
@@ -4065,7 +4071,7 @@
       <c r="M13" s="31"/>
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
+      <c r="P13" s="38"/>
       <c r="Q13" s="31" t="s">
         <v>49</v>
       </c>
@@ -4105,7 +4111,7 @@
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="31"/>
       <c r="R14" s="32"/>
       <c r="S14" s="33"/>
@@ -4157,8 +4163,8 @@
       <c r="O15" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P15" s="31" t="s">
-        <v>78</v>
+      <c r="P15" s="38" t="s">
+        <v>301</v>
       </c>
       <c r="Q15" s="31" t="s">
         <v>49</v>
@@ -4177,25 +4183,25 @@
         <v>44</v>
       </c>
       <c r="C16" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="E16" s="26" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>81</v>
       </c>
       <c r="F16" s="37">
         <v>44992</v>
       </c>
       <c r="G16" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="I16" s="37" t="s">
         <v>83</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>84</v>
       </c>
       <c r="J16" s="31" t="s">
         <v>48</v>
@@ -4208,13 +4214,13 @@
         <v>56</v>
       </c>
       <c r="N16" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O16" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P16" s="31" t="s">
-        <v>78</v>
+      <c r="P16" s="38" t="s">
+        <v>301</v>
       </c>
       <c r="Q16" s="31" t="s">
         <v>49</v>
@@ -4225,7 +4231,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>45</v>
       </c>
@@ -4236,10 +4242,10 @@
         <v>45</v>
       </c>
       <c r="D17" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="26" t="s">
         <v>86</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>87</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
@@ -4256,13 +4262,13 @@
         <v>48</v>
       </c>
       <c r="N17" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O17" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P17" s="31" t="s">
-        <v>89</v>
+      <c r="P17" s="38" t="s">
+        <v>301</v>
       </c>
       <c r="Q17" s="31" t="s">
         <v>49</v>
@@ -4284,22 +4290,22 @@
         <v>45</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" s="30">
         <v>44985</v>
       </c>
       <c r="G18" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="H18" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="30" t="s">
-        <v>94</v>
       </c>
       <c r="J18" s="31" t="s">
         <v>48</v>
@@ -4312,13 +4318,13 @@
         <v>56</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="O18" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="31" t="s">
-        <v>78</v>
+      <c r="P18" s="38" t="s">
+        <v>302</v>
       </c>
       <c r="Q18" s="31" t="s">
         <v>49</v>
@@ -4340,22 +4346,22 @@
         <v>45</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F19" s="30">
         <v>44985</v>
       </c>
       <c r="G19" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="30" t="s">
         <v>98</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="30" t="s">
-        <v>100</v>
       </c>
       <c r="J19" s="31" t="s">
         <v>48</v>
@@ -4368,13 +4374,13 @@
         <v>56</v>
       </c>
       <c r="N19" s="31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O19" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P19" s="31" t="s">
-        <v>78</v>
+      <c r="P19" s="38" t="s">
+        <v>302</v>
       </c>
       <c r="Q19" s="31" t="s">
         <v>49</v>
@@ -4396,22 +4402,22 @@
         <v>45</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F20" s="30">
         <v>44985</v>
       </c>
       <c r="G20" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="30" t="s">
         <v>104</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="I20" s="30" t="s">
-        <v>106</v>
       </c>
       <c r="J20" s="31" t="s">
         <v>48</v>
@@ -4424,13 +4430,13 @@
         <v>56</v>
       </c>
       <c r="N20" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O20" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P20" s="31" t="s">
-        <v>78</v>
+      <c r="P20" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q20" s="31" t="s">
         <v>49</v>
@@ -4452,22 +4458,22 @@
         <v>45</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F21" s="30">
         <v>44985</v>
       </c>
       <c r="G21" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="30" t="s">
         <v>110</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>112</v>
       </c>
       <c r="J21" s="31" t="s">
         <v>48</v>
@@ -4480,13 +4486,13 @@
         <v>56</v>
       </c>
       <c r="N21" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="31" t="s">
-        <v>78</v>
+      <c r="P21" s="38" t="s">
+        <v>302</v>
       </c>
       <c r="Q21" s="31" t="s">
         <v>49</v>
@@ -4508,22 +4514,22 @@
         <v>45</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F22" s="30">
         <v>44985</v>
       </c>
       <c r="G22" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="J22" s="31" t="s">
         <v>48</v>
@@ -4536,13 +4542,13 @@
         <v>56</v>
       </c>
       <c r="N22" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="O22" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P22" s="31" t="s">
-        <v>78</v>
+      <c r="P22" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q22" s="31" t="s">
         <v>49</v>
@@ -4564,22 +4570,22 @@
         <v>45</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F23" s="30">
         <v>44985</v>
       </c>
       <c r="G23" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" s="30" t="s">
         <v>122</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>124</v>
       </c>
       <c r="J23" s="31" t="s">
         <v>48</v>
@@ -4592,13 +4598,13 @@
         <v>56</v>
       </c>
       <c r="N23" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O23" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P23" s="31" t="s">
-        <v>78</v>
+      <c r="P23" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q23" s="31" t="s">
         <v>49</v>
@@ -4620,22 +4626,22 @@
         <v>45</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F24" s="30">
         <v>44985</v>
       </c>
       <c r="G24" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="H24" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="I24" s="30" t="s">
-        <v>130</v>
       </c>
       <c r="J24" s="31" t="s">
         <v>48</v>
@@ -4648,13 +4654,13 @@
         <v>56</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O24" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P24" s="31" t="s">
-        <v>78</v>
+      <c r="P24" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q24" s="31" t="s">
         <v>49</v>
@@ -4676,22 +4682,22 @@
         <v>45</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F25" s="30">
         <v>44985</v>
       </c>
       <c r="G25" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" s="30" t="s">
         <v>134</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="I25" s="30" t="s">
-        <v>136</v>
       </c>
       <c r="J25" s="31" t="s">
         <v>48</v>
@@ -4704,13 +4710,13 @@
         <v>56</v>
       </c>
       <c r="N25" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="O25" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P25" s="31" t="s">
-        <v>78</v>
+      <c r="P25" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q25" s="31" t="s">
         <v>49</v>
@@ -4732,22 +4738,22 @@
         <v>45</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F26" s="30">
         <v>44985</v>
       </c>
       <c r="G26" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" s="30" t="s">
         <v>140</v>
-      </c>
-      <c r="H26" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="I26" s="30" t="s">
-        <v>142</v>
       </c>
       <c r="J26" s="31" t="s">
         <v>48</v>
@@ -4760,13 +4766,13 @@
         <v>56</v>
       </c>
       <c r="N26" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O26" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P26" s="31" t="s">
-        <v>78</v>
+      <c r="P26" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q26" s="31" t="s">
         <v>49</v>
@@ -4788,10 +4794,10 @@
         <v>45</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
@@ -4807,7 +4813,7 @@
       <c r="M27" s="31"/>
       <c r="N27" s="31"/>
       <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="P27" s="38"/>
       <c r="Q27" s="31"/>
       <c r="R27" s="32"/>
       <c r="S27" s="33"/>
@@ -4826,22 +4832,22 @@
         <v>45</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F28" s="30">
         <v>44985</v>
       </c>
       <c r="G28" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="30" t="s">
         <v>148</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28" s="30" t="s">
-        <v>150</v>
       </c>
       <c r="J28" s="31" t="s">
         <v>48</v>
@@ -4854,13 +4860,13 @@
         <v>56</v>
       </c>
       <c r="N28" s="31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O28" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="P28" s="31" t="s">
-        <v>78</v>
+      <c r="P28" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q28" s="31" t="s">
         <v>49</v>
@@ -4882,10 +4888,10 @@
         <v>45</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -4901,7 +4907,7 @@
       <c r="M29" s="31"/>
       <c r="N29" s="31"/>
       <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
+      <c r="P29" s="38"/>
       <c r="Q29" s="31"/>
       <c r="R29" s="32"/>
       <c r="S29" s="33"/>
@@ -4917,25 +4923,25 @@
         <v>44</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="44" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E30" s="45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F30" s="46">
         <v>44992</v>
       </c>
       <c r="G30" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="I30" s="47" t="s">
         <v>156</v>
-      </c>
-      <c r="H30" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="I30" s="47" t="s">
-        <v>158</v>
       </c>
       <c r="J30" s="48" t="s">
         <v>48</v>
@@ -4945,7 +4951,7 @@
       <c r="M30" s="49"/>
       <c r="N30" s="49"/>
       <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
+      <c r="P30" s="38"/>
       <c r="Q30" s="48" t="s">
         <v>49</v>
       </c>
@@ -4963,13 +4969,13 @@
         <v>44</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" s="44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E31" s="45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F31" s="46"/>
       <c r="G31" s="47"/>
@@ -4985,7 +4991,7 @@
       <c r="M31" s="49"/>
       <c r="N31" s="49"/>
       <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
+      <c r="P31" s="38"/>
       <c r="Q31" s="48" t="s">
         <v>49</v>
       </c>
@@ -5003,13 +5009,13 @@
         <v>44</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E32" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F32" s="46"/>
       <c r="G32" s="47"/>
@@ -5025,7 +5031,7 @@
       <c r="M32" s="49"/>
       <c r="N32" s="49"/>
       <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
+      <c r="P32" s="38"/>
       <c r="Q32" s="48" t="s">
         <v>49</v>
       </c>
@@ -5043,13 +5049,13 @@
         <v>44</v>
       </c>
       <c r="C33" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" s="54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F33" s="56"/>
       <c r="G33" s="57"/>
@@ -5065,7 +5071,7 @@
       <c r="M33" s="57"/>
       <c r="N33" s="57"/>
       <c r="O33" s="57"/>
-      <c r="P33" s="57"/>
+      <c r="P33" s="38"/>
       <c r="Q33" s="57"/>
       <c r="R33" s="57"/>
       <c r="S33" s="58"/>
@@ -5081,25 +5087,25 @@
         <v>44</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F34" s="37">
         <v>44992</v>
       </c>
       <c r="G34" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="I34" s="37" t="s">
         <v>167</v>
-      </c>
-      <c r="H34" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="I34" s="37" t="s">
-        <v>169</v>
       </c>
       <c r="J34" s="31" t="s">
         <v>48</v>
@@ -5112,13 +5118,13 @@
         <v>56</v>
       </c>
       <c r="N34" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O34" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P34" s="31" t="s">
-        <v>78</v>
+      <c r="P34" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q34" s="31" t="s">
         <v>49</v>
@@ -5129,7 +5135,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36">
         <v>152</v>
       </c>
@@ -5137,25 +5143,25 @@
         <v>44</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F35" s="37">
         <v>44992</v>
       </c>
       <c r="G35" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H35" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="37" t="s">
         <v>173</v>
-      </c>
-      <c r="H35" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="I35" s="37" t="s">
-        <v>175</v>
       </c>
       <c r="J35" s="38" t="s">
         <v>48</v>
@@ -5168,13 +5174,13 @@
         <v>56</v>
       </c>
       <c r="N35" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="O35" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P35" s="31" t="s">
-        <v>78</v>
+      <c r="P35" s="38" t="s">
+        <v>304</v>
       </c>
       <c r="Q35" s="38"/>
       <c r="R35" s="32"/>
@@ -5191,25 +5197,25 @@
         <v>44</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="36" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F36" s="37">
         <v>44992</v>
       </c>
       <c r="G36" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="H36" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="I36" s="37" t="s">
         <v>179</v>
-      </c>
-      <c r="H36" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="I36" s="37" t="s">
-        <v>181</v>
       </c>
       <c r="J36" s="31" t="s">
         <v>48</v>
@@ -5222,13 +5228,13 @@
         <v>56</v>
       </c>
       <c r="N36" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="O36" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P36" s="31" t="s">
-        <v>78</v>
+      <c r="P36" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q36" s="31" t="s">
         <v>49</v>
@@ -5247,25 +5253,25 @@
         <v>44</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F37" s="37">
         <v>44992</v>
       </c>
       <c r="G37" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="I37" s="37" t="s">
         <v>185</v>
-      </c>
-      <c r="H37" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="I37" s="37" t="s">
-        <v>187</v>
       </c>
       <c r="J37" s="38" t="s">
         <v>48</v>
@@ -5278,13 +5284,13 @@
         <v>56</v>
       </c>
       <c r="N37" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="O37" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P37" s="31" t="s">
-        <v>78</v>
+      <c r="P37" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q37" s="31" t="s">
         <v>49</v>
@@ -5303,25 +5309,25 @@
         <v>44</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="36" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F38" s="37">
         <v>44992</v>
       </c>
       <c r="G38" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="I38" s="37" t="s">
         <v>191</v>
-      </c>
-      <c r="H38" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="I38" s="37" t="s">
-        <v>193</v>
       </c>
       <c r="J38" s="38" t="s">
         <v>48</v>
@@ -5334,13 +5340,13 @@
         <v>56</v>
       </c>
       <c r="N38" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O38" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P38" s="31" t="s">
-        <v>78</v>
+      <c r="P38" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q38" s="38" t="s">
         <v>49</v>
@@ -5359,25 +5365,25 @@
         <v>44</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E39" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F39" s="37">
         <v>44992</v>
       </c>
       <c r="G39" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="H39" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="I39" s="37" t="s">
         <v>197</v>
-      </c>
-      <c r="H39" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="I39" s="37" t="s">
-        <v>199</v>
       </c>
       <c r="J39" s="38" t="s">
         <v>48</v>
@@ -5390,13 +5396,13 @@
         <v>56</v>
       </c>
       <c r="N39" s="38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O39" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P39" s="31" t="s">
-        <v>78</v>
+      <c r="P39" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q39" s="38" t="s">
         <v>49</v>
@@ -5415,25 +5421,25 @@
         <v>44</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E40" s="41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F40" s="37">
         <v>44992</v>
       </c>
       <c r="G40" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="H40" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" s="37" t="s">
         <v>203</v>
-      </c>
-      <c r="H40" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="I40" s="37" t="s">
-        <v>205</v>
       </c>
       <c r="J40" s="38" t="s">
         <v>48</v>
@@ -5446,20 +5452,20 @@
         <v>56</v>
       </c>
       <c r="N40" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O40" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P40" s="31" t="s">
-        <v>78</v>
+      <c r="P40" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q40" s="38" t="s">
         <v>49</v>
       </c>
       <c r="R40" s="32"/>
       <c r="S40" s="41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T40" s="38" t="s">
         <v>71</v>
@@ -5473,25 +5479,25 @@
         <v>44</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41" s="36" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E41" s="41" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F41" s="37">
         <v>44992</v>
       </c>
       <c r="G41" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H41" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I41" s="37" t="s">
         <v>210</v>
-      </c>
-      <c r="H41" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="I41" s="37" t="s">
-        <v>212</v>
       </c>
       <c r="J41" s="38" t="s">
         <v>48</v>
@@ -5504,13 +5510,13 @@
         <v>56</v>
       </c>
       <c r="N41" s="38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="O41" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P41" s="31" t="s">
-        <v>78</v>
+      <c r="P41" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q41" s="38" t="s">
         <v>49</v>
@@ -5529,25 +5535,25 @@
         <v>44</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" s="36" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E42" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F42" s="37">
         <v>44992</v>
       </c>
       <c r="G42" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="H42" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="I42" s="37" t="s">
         <v>216</v>
-      </c>
-      <c r="H42" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="I42" s="37" t="s">
-        <v>218</v>
       </c>
       <c r="J42" s="38" t="s">
         <v>48</v>
@@ -5560,13 +5566,13 @@
         <v>56</v>
       </c>
       <c r="N42" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O42" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P42" s="31" t="s">
-        <v>78</v>
+      <c r="P42" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q42" s="38" t="s">
         <v>49</v>
@@ -5585,25 +5591,25 @@
         <v>44</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F43" s="37">
         <v>44992</v>
       </c>
       <c r="G43" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="H43" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="I43" s="37" t="s">
         <v>222</v>
-      </c>
-      <c r="H43" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="I43" s="37" t="s">
-        <v>224</v>
       </c>
       <c r="J43" s="38" t="s">
         <v>48</v>
@@ -5616,13 +5622,13 @@
         <v>56</v>
       </c>
       <c r="N43" s="38" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O43" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P43" s="31" t="s">
-        <v>78</v>
+      <c r="P43" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q43" s="38" t="s">
         <v>49</v>
@@ -5641,25 +5647,25 @@
         <v>44</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D44" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F44" s="37">
         <v>44992</v>
       </c>
       <c r="G44" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="I44" s="37" t="s">
         <v>228</v>
-      </c>
-      <c r="H44" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="I44" s="37" t="s">
-        <v>230</v>
       </c>
       <c r="J44" s="38" t="s">
         <v>48</v>
@@ -5672,13 +5678,13 @@
         <v>56</v>
       </c>
       <c r="N44" s="38" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O44" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P44" s="31" t="s">
-        <v>78</v>
+      <c r="P44" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q44" s="38" t="s">
         <v>49</v>
@@ -5697,25 +5703,25 @@
         <v>44</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D45" s="36" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E45" s="41" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F45" s="37">
         <v>44992</v>
       </c>
       <c r="G45" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="H45" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="I45" s="37" t="s">
         <v>234</v>
-      </c>
-      <c r="H45" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="I45" s="37" t="s">
-        <v>236</v>
       </c>
       <c r="J45" s="38" t="s">
         <v>48</v>
@@ -5728,13 +5734,13 @@
         <v>56</v>
       </c>
       <c r="N45" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O45" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P45" s="31" t="s">
-        <v>78</v>
+      <c r="P45" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q45" s="38" t="s">
         <v>49</v>
@@ -5753,25 +5759,25 @@
         <v>44</v>
       </c>
       <c r="C46" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E46" s="41" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F46" s="37">
         <v>44992</v>
       </c>
       <c r="G46" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="H46" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" s="37" t="s">
         <v>240</v>
-      </c>
-      <c r="H46" s="37" t="s">
-        <v>241</v>
-      </c>
-      <c r="I46" s="37" t="s">
-        <v>242</v>
       </c>
       <c r="J46" s="38" t="s">
         <v>48</v>
@@ -5784,13 +5790,13 @@
         <v>56</v>
       </c>
       <c r="N46" s="38" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O46" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P46" s="31" t="s">
-        <v>78</v>
+      <c r="P46" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q46" s="38" t="s">
         <v>49</v>
@@ -5809,25 +5815,25 @@
         <v>44</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F47" s="37">
         <v>44992</v>
       </c>
       <c r="G47" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="I47" s="37" t="s">
         <v>246</v>
-      </c>
-      <c r="H47" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="I47" s="37" t="s">
-        <v>248</v>
       </c>
       <c r="J47" s="38" t="s">
         <v>48</v>
@@ -5840,13 +5846,13 @@
         <v>56</v>
       </c>
       <c r="N47" s="38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O47" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P47" s="31" t="s">
-        <v>78</v>
+      <c r="P47" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q47" s="38" t="s">
         <v>49</v>
@@ -5865,25 +5871,25 @@
         <v>44</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E48" s="41" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F48" s="37">
         <v>44992</v>
       </c>
       <c r="G48" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="H48" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="I48" s="37" t="s">
         <v>252</v>
-      </c>
-      <c r="H48" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="I48" s="37" t="s">
-        <v>254</v>
       </c>
       <c r="J48" s="38" t="s">
         <v>48</v>
@@ -5896,13 +5902,13 @@
         <v>56</v>
       </c>
       <c r="N48" s="38" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O48" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P48" s="31" t="s">
-        <v>78</v>
+      <c r="P48" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q48" s="38"/>
       <c r="R48" s="32"/>
@@ -5919,13 +5925,13 @@
         <v>44</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E49" s="41" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F49" s="37"/>
       <c r="G49" s="37"/>
@@ -5934,22 +5940,12 @@
       <c r="J49" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="K49" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L49" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="M49" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="K49" s="31"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38"/>
       <c r="N49" s="38"/>
-      <c r="O49" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="P49" s="31" t="s">
-        <v>78</v>
-      </c>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
       <c r="Q49" s="38"/>
       <c r="R49" s="32"/>
       <c r="S49" s="42"/>
@@ -5965,13 +5961,13 @@
         <v>44</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F50" s="37"/>
       <c r="G50" s="37"/>
@@ -5980,22 +5976,12 @@
       <c r="J50" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="K50" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L50" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="M50" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="K50" s="31"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
       <c r="N50" s="38"/>
-      <c r="O50" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="P50" s="31" t="s">
-        <v>78</v>
-      </c>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
       <c r="Q50" s="38"/>
       <c r="R50" s="32"/>
       <c r="S50" s="42"/>
@@ -6011,25 +5997,25 @@
         <v>44</v>
       </c>
       <c r="C51" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F51" s="37">
         <v>44992</v>
       </c>
       <c r="G51" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="H51" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="I51" s="37" t="s">
         <v>262</v>
-      </c>
-      <c r="H51" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="I51" s="37" t="s">
-        <v>264</v>
       </c>
       <c r="J51" s="38" t="s">
         <v>48</v>
@@ -6042,13 +6028,13 @@
         <v>56</v>
       </c>
       <c r="N51" s="38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O51" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P51" s="31" t="s">
-        <v>78</v>
+      <c r="P51" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q51" s="38" t="s">
         <v>49</v>
@@ -6067,25 +6053,25 @@
         <v>44</v>
       </c>
       <c r="C52" s="36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D52" s="36" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E52" s="41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F52" s="37">
         <v>44992</v>
       </c>
       <c r="G52" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="H52" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="I52" s="37" t="s">
         <v>268</v>
-      </c>
-      <c r="H52" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="I52" s="37" t="s">
-        <v>270</v>
       </c>
       <c r="J52" s="38" t="s">
         <v>48</v>
@@ -6098,13 +6084,13 @@
         <v>56</v>
       </c>
       <c r="N52" s="38" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O52" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P52" s="31" t="s">
-        <v>78</v>
+      <c r="P52" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="Q52" s="38" t="s">
         <v>49</v>
@@ -20105,7 +20091,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7251B2DD-EAA3-474F-9C39-00147BB6DBBD}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
@@ -20156,24 +20142,24 @@
         <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>275</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20181,111 +20167,111 @@
         <v>45</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>280</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>283</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>286</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>287</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>289</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>294</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C10" s="23">
         <v>191</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21313,7 +21299,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B3" s="61" t="s">
         <v>56</v>
@@ -22330,6 +22316,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DFBE386201AE734F9EC9E17D4E3DD9C4" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="5f97ab7aa040c3457a612e608e5ad366">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce" xmlns:ns3="3560cf22-a742-4796-b196-7e41d1f38b33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="47906dabeb809e6ed6721806972ae013" ns2:_="" ns3:_="">
     <xsd:import namespace="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
@@ -22572,27 +22578,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
+    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3560cf22-a742-4796-b196-7e41d1f38b33" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6F8571-9F7A-4376-AF4F-C06E7C571BAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22611,25 +22616,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3560cf22-a742-4796-b196-7e41d1f38b33"/>
-    <ds:schemaRef ds:uri="75a0c07b-716c-4c90-8f3d-6a9bd2d886ce"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>